<commit_message>
experimented with unicodedata module and classifying diacritics
</commit_message>
<xml_diff>
--- a/misc/4th_canon_master.xlsx
+++ b/misc/4th_canon_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46b70eb444d7c99a/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiveseher/Documents/GitHub-Repositories/neologos/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="252" documentId="8_{A1E9936A-B030-8C41-B0C6-FE4D7CA7F608}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{BA045DCE-AB08-ED47-83E1-2C8F3FB0689C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76E5B76-DDEC-6143-8E36-F58D3942948E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="28200" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="28200" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phonetics" sheetId="2" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="Dictionary" sheetId="29" r:id="rId4"/>
     <sheet name="Basics" sheetId="10" r:id="rId5"/>
     <sheet name="Conjugation" sheetId="13" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="31" r:id="rId7"/>
-    <sheet name="Idioms" sheetId="19" r:id="rId8"/>
+    <sheet name="Idioms" sheetId="19" r:id="rId7"/>
+    <sheet name="Ph. Change (2)" sheetId="32" r:id="rId8"/>
     <sheet name="Ph. Change" sheetId="11" r:id="rId9"/>
     <sheet name="Sem. Change" sheetId="25" r:id="rId10"/>
     <sheet name="OldConjChart" sheetId="21" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Dictionary!$A$1:$T$590</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="7" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="1045">
   <si>
     <t>person</t>
   </si>
@@ -4265,6 +4266,162 @@
   </si>
   <si>
     <t>ʀiɳ.çi.rin.jia</t>
+  </si>
+  <si>
+    <t>amra &gt; ambra</t>
+  </si>
+  <si>
+    <t>asata &gt; atasa</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Optional conditions</t>
+  </si>
+  <si>
+    <t>+OPEN_VOWELS</t>
+  </si>
+  <si>
+    <t>+LOWER_VOWELS</t>
+  </si>
+  <si>
+    <t>-DUPLICATE</t>
+  </si>
+  <si>
+    <t>+DUPLICATE</t>
+  </si>
+  <si>
+    <t>+POLYPHTHONG</t>
+  </si>
+  <si>
+    <t>-POLYPHTHONG</t>
+  </si>
+  <si>
+    <t>+VOICED</t>
+  </si>
+  <si>
+    <t>-VOICED</t>
+  </si>
+  <si>
+    <t>Obligatory environment</t>
+  </si>
+  <si>
+    <t>Optional environment</t>
+  </si>
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t>Step 2</t>
+  </si>
+  <si>
+    <t>Step 3</t>
+  </si>
+  <si>
+    <t>-ELEMENT</t>
+  </si>
+  <si>
+    <t>-AFFRICATE</t>
+  </si>
+  <si>
+    <t>+AFFRICATE</t>
+  </si>
+  <si>
+    <t>+NASAL</t>
+  </si>
+  <si>
+    <t>+LENGTH</t>
+  </si>
+  <si>
+    <t>-LENGTH</t>
+  </si>
+  <si>
+    <t>+PALATAL</t>
+  </si>
+  <si>
+    <t>+PLACE_OF_NEXT</t>
+  </si>
+  <si>
+    <t>+FRICATIVE</t>
+  </si>
+  <si>
+    <t>+PLACE_OF_LAST</t>
+  </si>
+  <si>
+    <t>+ELEMENT</t>
+  </si>
+  <si>
+    <t>VOWEL</t>
+  </si>
+  <si>
+    <t>INITIAL</t>
+  </si>
+  <si>
+    <t>FINAL</t>
+  </si>
+  <si>
+    <t>MEDIAL *</t>
+  </si>
+  <si>
+    <t>Related</t>
+  </si>
+  <si>
+    <t>INTERVOCALIC</t>
+  </si>
+  <si>
+    <t>INTERCONSONANTAL</t>
+  </si>
+  <si>
+    <t>CONSONANT</t>
+  </si>
+  <si>
+    <t>VOWEL (POLYPHTHONG)</t>
+  </si>
+  <si>
+    <t>CONSONANT (DUPLICATED)</t>
+  </si>
+  <si>
+    <t>SEQUENCE (DUPLICATED)</t>
+  </si>
+  <si>
+    <t>NASAL CONSONANT</t>
+  </si>
+  <si>
+    <t>ANY (USUALLY VOWEL)</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Obligatory element (INPUT)</t>
+  </si>
+  <si>
+    <t>Obligatory element (OUTPUT)</t>
+  </si>
+  <si>
+    <t>SYLLABLE BOUNDARY</t>
+  </si>
+  <si>
+    <t>POST-DELETION</t>
+  </si>
+  <si>
+    <t>/s/ or /z/</t>
+  </si>
+  <si>
+    <t>INTERVOCALIC OR INTERGLIDE</t>
+  </si>
+  <si>
+    <t>/r/</t>
+  </si>
+  <si>
+    <t>+SONORITY</t>
+  </si>
+  <si>
+    <t>Palatalization</t>
+  </si>
+  <si>
+    <t>k &gt; tʃ; t &gt; tʃ; s &gt; ʃ; s &gt; s</t>
   </si>
 </sst>
 </file>
@@ -7485,7 +7642,7 @@
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="442">
+  <cellXfs count="448">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8133,28 +8290,18 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="925" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -8163,11 +8310,23 @@
     <xf numFmtId="49" fontId="25" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8208,8 +8367,16 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="650" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="925" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="926">
     <cellStyle name="40% - Accent6" xfId="649" builtinId="51"/>
@@ -9141,6 +9308,55 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color indexed="64"/>
@@ -9249,55 +9465,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -9568,12 +9735,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:C27" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:C27" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:C27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="literal translation" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="meaning" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="translation" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="literal translation" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="meaning" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="translation" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10425,84 +10592,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="C1" s="430" t="s">
+      <c r="C1" s="432" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="431"/>
-      <c r="E1" s="431"/>
-      <c r="F1" s="431"/>
-      <c r="G1" s="431"/>
-      <c r="H1" s="431"/>
-      <c r="I1" s="431"/>
-      <c r="J1" s="431"/>
-      <c r="K1" s="431"/>
-      <c r="L1" s="431"/>
-      <c r="M1" s="431"/>
-      <c r="N1" s="431"/>
-      <c r="O1" s="431"/>
-      <c r="P1" s="431"/>
-      <c r="Q1" s="431"/>
-      <c r="R1" s="431"/>
-      <c r="S1" s="431"/>
-      <c r="T1" s="432"/>
+      <c r="D1" s="433"/>
+      <c r="E1" s="433"/>
+      <c r="F1" s="433"/>
+      <c r="G1" s="433"/>
+      <c r="H1" s="433"/>
+      <c r="I1" s="433"/>
+      <c r="J1" s="433"/>
+      <c r="K1" s="433"/>
+      <c r="L1" s="433"/>
+      <c r="M1" s="433"/>
+      <c r="N1" s="433"/>
+      <c r="O1" s="433"/>
+      <c r="P1" s="433"/>
+      <c r="Q1" s="433"/>
+      <c r="R1" s="433"/>
+      <c r="S1" s="433"/>
+      <c r="T1" s="434"/>
     </row>
     <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
-      <c r="C2" s="433" t="s">
+      <c r="C2" s="435" t="s">
         <v>282</v>
       </c>
-      <c r="D2" s="434"/>
-      <c r="E2" s="434"/>
-      <c r="F2" s="434"/>
-      <c r="G2" s="434"/>
-      <c r="H2" s="434"/>
-      <c r="I2" s="434"/>
-      <c r="J2" s="434"/>
-      <c r="K2" s="434"/>
-      <c r="L2" s="434"/>
-      <c r="M2" s="434"/>
-      <c r="N2" s="434"/>
-      <c r="O2" s="434"/>
-      <c r="P2" s="434"/>
-      <c r="Q2" s="434"/>
-      <c r="R2" s="434"/>
-      <c r="S2" s="434"/>
-      <c r="T2" s="435"/>
+      <c r="D2" s="436"/>
+      <c r="E2" s="436"/>
+      <c r="F2" s="436"/>
+      <c r="G2" s="436"/>
+      <c r="H2" s="436"/>
+      <c r="I2" s="436"/>
+      <c r="J2" s="436"/>
+      <c r="K2" s="436"/>
+      <c r="L2" s="436"/>
+      <c r="M2" s="436"/>
+      <c r="N2" s="436"/>
+      <c r="O2" s="436"/>
+      <c r="P2" s="436"/>
+      <c r="Q2" s="436"/>
+      <c r="R2" s="436"/>
+      <c r="S2" s="436"/>
+      <c r="T2" s="437"/>
     </row>
     <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="436" t="s">
+      <c r="C3" s="438" t="s">
         <v>283</v>
       </c>
-      <c r="D3" s="437"/>
-      <c r="E3" s="438"/>
-      <c r="F3" s="437" t="s">
+      <c r="D3" s="439"/>
+      <c r="E3" s="440"/>
+      <c r="F3" s="439" t="s">
         <v>284</v>
       </c>
-      <c r="G3" s="437"/>
-      <c r="H3" s="439"/>
-      <c r="I3" s="437" t="s">
+      <c r="G3" s="439"/>
+      <c r="H3" s="441"/>
+      <c r="I3" s="439" t="s">
         <v>285</v>
       </c>
-      <c r="J3" s="437"/>
-      <c r="K3" s="439"/>
-      <c r="L3" s="437" t="s">
+      <c r="J3" s="439"/>
+      <c r="K3" s="441"/>
+      <c r="L3" s="439" t="s">
         <v>286</v>
       </c>
-      <c r="M3" s="437"/>
-      <c r="N3" s="439"/>
-      <c r="O3" s="437" t="s">
+      <c r="M3" s="439"/>
+      <c r="N3" s="441"/>
+      <c r="O3" s="439" t="s">
         <v>287</v>
       </c>
-      <c r="P3" s="437"/>
-      <c r="Q3" s="439"/>
-      <c r="R3" s="437" t="s">
+      <c r="P3" s="439"/>
+      <c r="Q3" s="441"/>
+      <c r="R3" s="439" t="s">
         <v>288</v>
       </c>
-      <c r="S3" s="437"/>
-      <c r="T3" s="438"/>
+      <c r="S3" s="439"/>
+      <c r="T3" s="440"/>
     </row>
     <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
@@ -11481,7 +11648,7 @@
   <dimension ref="B1:AS34"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="R23" sqref="R23:AO34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11512,47 +11679,47 @@
     </row>
     <row r="2" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
-      <c r="C2" s="425" t="s">
+      <c r="C2" s="417" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="425"/>
-      <c r="E2" s="425"/>
-      <c r="F2" s="425"/>
-      <c r="G2" s="425"/>
-      <c r="H2" s="425"/>
-      <c r="I2" s="425"/>
-      <c r="J2" s="425"/>
-      <c r="K2" s="425"/>
-      <c r="L2" s="425"/>
-      <c r="M2" s="425"/>
-      <c r="N2" s="425"/>
-      <c r="O2" s="425"/>
-      <c r="P2" s="425"/>
-      <c r="Q2" s="425"/>
-      <c r="R2" s="425"/>
-      <c r="S2" s="425"/>
-      <c r="T2" s="425"/>
-      <c r="U2" s="425"/>
-      <c r="V2" s="425"/>
-      <c r="W2" s="425"/>
-      <c r="X2" s="425"/>
-      <c r="Y2" s="425"/>
-      <c r="Z2" s="425"/>
-      <c r="AA2" s="425"/>
-      <c r="AB2" s="425"/>
-      <c r="AC2" s="425"/>
-      <c r="AD2" s="425"/>
-      <c r="AE2" s="425"/>
-      <c r="AF2" s="425"/>
-      <c r="AG2" s="425"/>
-      <c r="AH2" s="425"/>
-      <c r="AI2" s="425"/>
-      <c r="AJ2" s="425"/>
-      <c r="AK2" s="425"/>
-      <c r="AL2" s="425"/>
-      <c r="AM2" s="425"/>
-      <c r="AN2" s="425"/>
-      <c r="AO2" s="425"/>
+      <c r="D2" s="417"/>
+      <c r="E2" s="417"/>
+      <c r="F2" s="417"/>
+      <c r="G2" s="417"/>
+      <c r="H2" s="417"/>
+      <c r="I2" s="417"/>
+      <c r="J2" s="417"/>
+      <c r="K2" s="417"/>
+      <c r="L2" s="417"/>
+      <c r="M2" s="417"/>
+      <c r="N2" s="417"/>
+      <c r="O2" s="417"/>
+      <c r="P2" s="417"/>
+      <c r="Q2" s="417"/>
+      <c r="R2" s="417"/>
+      <c r="S2" s="417"/>
+      <c r="T2" s="417"/>
+      <c r="U2" s="417"/>
+      <c r="V2" s="417"/>
+      <c r="W2" s="417"/>
+      <c r="X2" s="417"/>
+      <c r="Y2" s="417"/>
+      <c r="Z2" s="417"/>
+      <c r="AA2" s="417"/>
+      <c r="AB2" s="417"/>
+      <c r="AC2" s="417"/>
+      <c r="AD2" s="417"/>
+      <c r="AE2" s="417"/>
+      <c r="AF2" s="417"/>
+      <c r="AG2" s="417"/>
+      <c r="AH2" s="417"/>
+      <c r="AI2" s="417"/>
+      <c r="AJ2" s="417"/>
+      <c r="AK2" s="417"/>
+      <c r="AL2" s="417"/>
+      <c r="AM2" s="417"/>
+      <c r="AN2" s="417"/>
+      <c r="AO2" s="417"/>
     </row>
     <row r="3" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
@@ -11588,59 +11755,59 @@
       <c r="Q4" s="353" t="s">
         <v>532</v>
       </c>
-      <c r="R4" s="422" t="s">
+      <c r="R4" s="418" t="s">
         <v>533</v>
       </c>
-      <c r="S4" s="422"/>
-      <c r="T4" s="422"/>
-      <c r="U4" s="422"/>
-      <c r="V4" s="422"/>
-      <c r="W4" s="422" t="s">
+      <c r="S4" s="418"/>
+      <c r="T4" s="418"/>
+      <c r="U4" s="418"/>
+      <c r="V4" s="418"/>
+      <c r="W4" s="418" t="s">
         <v>534</v>
       </c>
-      <c r="X4" s="422"/>
-      <c r="Y4" s="422"/>
-      <c r="Z4" s="422"/>
-      <c r="AA4" s="422"/>
-      <c r="AB4" s="422"/>
-      <c r="AC4" s="422"/>
-      <c r="AD4" s="422"/>
-      <c r="AE4" s="422"/>
-      <c r="AF4" s="422"/>
-      <c r="AG4" s="422" t="s">
+      <c r="X4" s="418"/>
+      <c r="Y4" s="418"/>
+      <c r="Z4" s="418"/>
+      <c r="AA4" s="418"/>
+      <c r="AB4" s="418"/>
+      <c r="AC4" s="418"/>
+      <c r="AD4" s="418"/>
+      <c r="AE4" s="418"/>
+      <c r="AF4" s="418"/>
+      <c r="AG4" s="418" t="s">
         <v>535</v>
       </c>
-      <c r="AH4" s="422"/>
-      <c r="AI4" s="422"/>
-      <c r="AJ4" s="422"/>
-      <c r="AK4" s="422"/>
-      <c r="AL4" s="422" t="s">
+      <c r="AH4" s="418"/>
+      <c r="AI4" s="418"/>
+      <c r="AJ4" s="418"/>
+      <c r="AK4" s="418"/>
+      <c r="AL4" s="418" t="s">
         <v>536</v>
       </c>
-      <c r="AM4" s="422"/>
-      <c r="AN4" s="422"/>
-      <c r="AO4" s="422"/>
+      <c r="AM4" s="418"/>
+      <c r="AN4" s="418"/>
+      <c r="AO4" s="418"/>
       <c r="AR4" s="32"/>
       <c r="AS4" s="32"/>
     </row>
     <row r="5" spans="2:45" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="313"/>
-      <c r="C5" s="426" t="s">
+      <c r="C5" s="420" t="s">
         <v>884</v>
       </c>
-      <c r="D5" s="426"/>
+      <c r="D5" s="420"/>
       <c r="E5" s="314"/>
       <c r="F5" s="314"/>
-      <c r="G5" s="426" t="s">
+      <c r="G5" s="420" t="s">
         <v>885</v>
       </c>
-      <c r="H5" s="426"/>
+      <c r="H5" s="420"/>
       <c r="I5" s="314"/>
       <c r="J5" s="314"/>
-      <c r="K5" s="426" t="s">
+      <c r="K5" s="420" t="s">
         <v>886</v>
       </c>
-      <c r="L5" s="426"/>
+      <c r="L5" s="420"/>
       <c r="M5" s="313"/>
       <c r="N5" s="313"/>
       <c r="O5" s="314"/>
@@ -11648,54 +11815,54 @@
       <c r="Q5" s="353" t="s">
         <v>537</v>
       </c>
-      <c r="R5" s="420" t="s">
+      <c r="R5" s="419" t="s">
         <v>538</v>
       </c>
-      <c r="S5" s="420"/>
-      <c r="T5" s="420" t="s">
+      <c r="S5" s="419"/>
+      <c r="T5" s="419" t="s">
         <v>539</v>
       </c>
-      <c r="U5" s="420"/>
-      <c r="V5" s="420" t="s">
+      <c r="U5" s="419"/>
+      <c r="V5" s="419" t="s">
         <v>540</v>
       </c>
-      <c r="W5" s="420"/>
-      <c r="X5" s="420" t="s">
+      <c r="W5" s="419"/>
+      <c r="X5" s="419" t="s">
         <v>541</v>
       </c>
-      <c r="Y5" s="420"/>
-      <c r="Z5" s="420" t="s">
+      <c r="Y5" s="419"/>
+      <c r="Z5" s="419" t="s">
         <v>542</v>
       </c>
-      <c r="AA5" s="420"/>
-      <c r="AB5" s="420" t="s">
+      <c r="AA5" s="419"/>
+      <c r="AB5" s="419" t="s">
         <v>543</v>
       </c>
-      <c r="AC5" s="420"/>
-      <c r="AD5" s="420" t="s">
+      <c r="AC5" s="419"/>
+      <c r="AD5" s="419" t="s">
         <v>544</v>
       </c>
-      <c r="AE5" s="420"/>
-      <c r="AF5" s="420" t="s">
+      <c r="AE5" s="419"/>
+      <c r="AF5" s="419" t="s">
         <v>545</v>
       </c>
-      <c r="AG5" s="420"/>
-      <c r="AH5" s="420" t="s">
+      <c r="AG5" s="419"/>
+      <c r="AH5" s="419" t="s">
         <v>546</v>
       </c>
-      <c r="AI5" s="420"/>
-      <c r="AJ5" s="420" t="s">
+      <c r="AI5" s="419"/>
+      <c r="AJ5" s="419" t="s">
         <v>547</v>
       </c>
-      <c r="AK5" s="420"/>
-      <c r="AL5" s="424" t="s">
+      <c r="AK5" s="419"/>
+      <c r="AL5" s="422" t="s">
         <v>648</v>
       </c>
-      <c r="AM5" s="424"/>
-      <c r="AN5" s="420" t="s">
+      <c r="AM5" s="422"/>
+      <c r="AN5" s="419" t="s">
         <v>548</v>
       </c>
-      <c r="AO5" s="420"/>
+      <c r="AO5" s="419"/>
       <c r="AR5" s="32"/>
       <c r="AS5" s="32"/>
     </row>
@@ -12652,582 +12819,703 @@
     <row r="21" spans="2:41" x14ac:dyDescent="0.2">
       <c r="P21" s="411"/>
       <c r="Q21" s="412"/>
-      <c r="R21" s="422" t="s">
+      <c r="R21" s="418" t="s">
         <v>533</v>
       </c>
-      <c r="S21" s="422"/>
-      <c r="T21" s="422"/>
-      <c r="U21" s="422"/>
-      <c r="V21" s="422"/>
-      <c r="W21" s="422" t="s">
+      <c r="S21" s="418"/>
+      <c r="T21" s="418"/>
+      <c r="U21" s="418"/>
+      <c r="V21" s="418"/>
+      <c r="W21" s="418" t="s">
         <v>534</v>
       </c>
-      <c r="X21" s="422"/>
-      <c r="Y21" s="422"/>
-      <c r="Z21" s="422"/>
-      <c r="AA21" s="422"/>
-      <c r="AB21" s="422"/>
-      <c r="AC21" s="422"/>
-      <c r="AD21" s="422"/>
-      <c r="AE21" s="422"/>
-      <c r="AF21" s="422"/>
-      <c r="AG21" s="422" t="s">
+      <c r="X21" s="418"/>
+      <c r="Y21" s="418"/>
+      <c r="Z21" s="418"/>
+      <c r="AA21" s="418"/>
+      <c r="AB21" s="418"/>
+      <c r="AC21" s="418"/>
+      <c r="AD21" s="418"/>
+      <c r="AE21" s="418"/>
+      <c r="AF21" s="418"/>
+      <c r="AG21" s="418" t="s">
         <v>535</v>
       </c>
-      <c r="AH21" s="422"/>
-      <c r="AI21" s="422"/>
-      <c r="AJ21" s="422"/>
-      <c r="AK21" s="422"/>
-      <c r="AL21" s="422" t="s">
+      <c r="AH21" s="418"/>
+      <c r="AI21" s="418"/>
+      <c r="AJ21" s="418"/>
+      <c r="AK21" s="418"/>
+      <c r="AL21" s="418" t="s">
         <v>536</v>
       </c>
-      <c r="AM21" s="422"/>
-      <c r="AN21" s="422"/>
-      <c r="AO21" s="422"/>
+      <c r="AM21" s="418"/>
+      <c r="AN21" s="418"/>
+      <c r="AO21" s="418"/>
     </row>
     <row r="22" spans="2:41" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P22" s="411"/>
       <c r="Q22" s="413"/>
-      <c r="R22" s="420" t="s">
+      <c r="R22" s="419" t="s">
         <v>538</v>
       </c>
-      <c r="S22" s="420"/>
-      <c r="T22" s="420" t="s">
+      <c r="S22" s="419"/>
+      <c r="T22" s="419" t="s">
         <v>539</v>
       </c>
-      <c r="U22" s="420"/>
-      <c r="V22" s="420" t="s">
+      <c r="U22" s="419"/>
+      <c r="V22" s="419" t="s">
         <v>540</v>
       </c>
-      <c r="W22" s="420"/>
-      <c r="X22" s="420" t="s">
+      <c r="W22" s="419"/>
+      <c r="X22" s="419" t="s">
         <v>541</v>
       </c>
-      <c r="Y22" s="420"/>
-      <c r="Z22" s="420" t="s">
+      <c r="Y22" s="419"/>
+      <c r="Z22" s="419" t="s">
         <v>542</v>
       </c>
-      <c r="AA22" s="420"/>
-      <c r="AB22" s="420" t="s">
+      <c r="AA22" s="419"/>
+      <c r="AB22" s="419" t="s">
         <v>543</v>
       </c>
-      <c r="AC22" s="420"/>
-      <c r="AD22" s="420" t="s">
+      <c r="AC22" s="419"/>
+      <c r="AD22" s="419" t="s">
         <v>544</v>
       </c>
-      <c r="AE22" s="420"/>
-      <c r="AF22" s="420" t="s">
+      <c r="AE22" s="419"/>
+      <c r="AF22" s="419" t="s">
         <v>545</v>
       </c>
-      <c r="AG22" s="420"/>
-      <c r="AH22" s="420" t="s">
+      <c r="AG22" s="419"/>
+      <c r="AH22" s="419" t="s">
         <v>546</v>
       </c>
-      <c r="AI22" s="420"/>
-      <c r="AJ22" s="420" t="s">
+      <c r="AI22" s="419"/>
+      <c r="AJ22" s="419" t="s">
         <v>547</v>
       </c>
-      <c r="AK22" s="420"/>
-      <c r="AL22" s="421" t="s">
+      <c r="AK22" s="419"/>
+      <c r="AL22" s="426" t="s">
         <v>648</v>
       </c>
-      <c r="AM22" s="421"/>
-      <c r="AN22" s="420" t="s">
+      <c r="AM22" s="426"/>
+      <c r="AN22" s="419" t="s">
         <v>548</v>
       </c>
-      <c r="AO22" s="420"/>
+      <c r="AO22" s="419"/>
     </row>
     <row r="23" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P23" s="423" t="s">
+      <c r="P23" s="421" t="s">
         <v>649</v>
       </c>
       <c r="Q23" s="412" t="s">
         <v>556</v>
       </c>
-      <c r="R23" s="418" t="s">
+      <c r="R23" s="423" t="s">
         <v>650</v>
       </c>
-      <c r="S23" s="418"/>
-      <c r="T23" s="419"/>
-      <c r="U23" s="419"/>
-      <c r="V23" s="415"/>
-      <c r="W23" s="415"/>
-      <c r="X23" s="419"/>
-      <c r="Y23" s="419"/>
-      <c r="Z23" s="418" t="s">
+      <c r="S23" s="423"/>
+      <c r="T23" s="424"/>
+      <c r="U23" s="424"/>
+      <c r="V23" s="425"/>
+      <c r="W23" s="425"/>
+      <c r="X23" s="424"/>
+      <c r="Y23" s="424"/>
+      <c r="Z23" s="423" t="s">
         <v>651</v>
       </c>
-      <c r="AA23" s="418"/>
-      <c r="AB23" s="419"/>
-      <c r="AC23" s="419"/>
-      <c r="AD23" s="418" t="s">
+      <c r="AA23" s="423"/>
+      <c r="AB23" s="424"/>
+      <c r="AC23" s="424"/>
+      <c r="AD23" s="423" t="s">
         <v>652</v>
       </c>
-      <c r="AE23" s="418"/>
-      <c r="AF23" s="418" t="s">
+      <c r="AE23" s="423"/>
+      <c r="AF23" s="423" t="s">
         <v>653</v>
       </c>
-      <c r="AG23" s="418"/>
-      <c r="AH23" s="418" t="s">
+      <c r="AG23" s="423"/>
+      <c r="AH23" s="423" t="s">
         <v>654</v>
       </c>
-      <c r="AI23" s="418"/>
-      <c r="AJ23" s="418" t="s">
+      <c r="AI23" s="423"/>
+      <c r="AJ23" s="423" t="s">
         <v>655</v>
       </c>
-      <c r="AK23" s="418"/>
-      <c r="AL23" s="418" t="s">
+      <c r="AK23" s="423"/>
+      <c r="AL23" s="423" t="s">
         <v>656</v>
       </c>
-      <c r="AM23" s="418"/>
-      <c r="AN23" s="416"/>
-      <c r="AO23" s="416"/>
+      <c r="AM23" s="423"/>
+      <c r="AN23" s="427"/>
+      <c r="AO23" s="427"/>
     </row>
     <row r="24" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P24" s="423"/>
+      <c r="P24" s="421"/>
       <c r="Q24" s="412" t="s">
         <v>657</v>
       </c>
-      <c r="R24" s="419"/>
-      <c r="S24" s="419"/>
-      <c r="T24" s="415"/>
-      <c r="U24" s="415"/>
-      <c r="V24" s="415"/>
-      <c r="W24" s="415"/>
-      <c r="X24" s="418" t="s">
+      <c r="R24" s="424"/>
+      <c r="S24" s="424"/>
+      <c r="T24" s="425"/>
+      <c r="U24" s="425"/>
+      <c r="V24" s="425"/>
+      <c r="W24" s="425"/>
+      <c r="X24" s="423" t="s">
         <v>658</v>
       </c>
-      <c r="Y24" s="418"/>
-      <c r="Z24" s="418" t="s">
+      <c r="Y24" s="423"/>
+      <c r="Z24" s="423" t="s">
         <v>659</v>
       </c>
-      <c r="AA24" s="418"/>
-      <c r="AB24" s="418" t="s">
+      <c r="AA24" s="423"/>
+      <c r="AB24" s="423" t="s">
         <v>660</v>
       </c>
-      <c r="AC24" s="418"/>
-      <c r="AD24" s="418" t="s">
+      <c r="AC24" s="423"/>
+      <c r="AD24" s="423" t="s">
         <v>661</v>
       </c>
-      <c r="AE24" s="418"/>
-      <c r="AF24" s="419"/>
-      <c r="AG24" s="419"/>
-      <c r="AH24" s="418" t="s">
+      <c r="AE24" s="423"/>
+      <c r="AF24" s="424"/>
+      <c r="AG24" s="424"/>
+      <c r="AH24" s="423" t="s">
         <v>662</v>
       </c>
-      <c r="AI24" s="418"/>
-      <c r="AJ24" s="418" t="s">
+      <c r="AI24" s="423"/>
+      <c r="AJ24" s="423" t="s">
         <v>663</v>
       </c>
-      <c r="AK24" s="418"/>
-      <c r="AL24" s="419"/>
-      <c r="AM24" s="419"/>
-      <c r="AN24" s="416"/>
-      <c r="AO24" s="416"/>
+      <c r="AK24" s="423"/>
+      <c r="AL24" s="424"/>
+      <c r="AM24" s="424"/>
+      <c r="AN24" s="427"/>
+      <c r="AO24" s="427"/>
     </row>
     <row r="25" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P25" s="423"/>
+      <c r="P25" s="421"/>
       <c r="Q25" s="412" t="s">
         <v>664</v>
       </c>
-      <c r="R25" s="418" t="s">
+      <c r="R25" s="423" t="s">
         <v>665</v>
       </c>
-      <c r="S25" s="418"/>
-      <c r="T25" s="418" t="s">
+      <c r="S25" s="423"/>
+      <c r="T25" s="423" t="s">
         <v>666</v>
       </c>
-      <c r="U25" s="418"/>
-      <c r="V25" s="416"/>
-      <c r="W25" s="416"/>
-      <c r="X25" s="418" t="s">
+      <c r="U25" s="423"/>
+      <c r="V25" s="427"/>
+      <c r="W25" s="427"/>
+      <c r="X25" s="423" t="s">
         <v>667</v>
       </c>
-      <c r="Y25" s="418"/>
-      <c r="Z25" s="418" t="s">
+      <c r="Y25" s="423"/>
+      <c r="Z25" s="423" t="s">
         <v>668</v>
       </c>
-      <c r="AA25" s="418"/>
-      <c r="AB25" s="418" t="s">
+      <c r="AA25" s="423"/>
+      <c r="AB25" s="423" t="s">
         <v>669</v>
       </c>
-      <c r="AC25" s="418"/>
-      <c r="AD25" s="418" t="s">
+      <c r="AC25" s="423"/>
+      <c r="AD25" s="423" t="s">
         <v>670</v>
       </c>
-      <c r="AE25" s="418"/>
-      <c r="AF25" s="418" t="s">
+      <c r="AE25" s="423"/>
+      <c r="AF25" s="423" t="s">
         <v>671</v>
       </c>
-      <c r="AG25" s="418"/>
-      <c r="AH25" s="418" t="s">
+      <c r="AG25" s="423"/>
+      <c r="AH25" s="423" t="s">
         <v>672</v>
       </c>
-      <c r="AI25" s="418"/>
-      <c r="AJ25" s="418" t="s">
+      <c r="AI25" s="423"/>
+      <c r="AJ25" s="423" t="s">
         <v>673</v>
       </c>
-      <c r="AK25" s="418"/>
-      <c r="AL25" s="415"/>
-      <c r="AM25" s="415"/>
-      <c r="AN25" s="417"/>
-      <c r="AO25" s="417"/>
+      <c r="AK25" s="423"/>
+      <c r="AL25" s="425"/>
+      <c r="AM25" s="425"/>
+      <c r="AN25" s="428"/>
+      <c r="AO25" s="428"/>
     </row>
     <row r="26" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P26" s="423"/>
+      <c r="P26" s="421"/>
       <c r="Q26" s="412" t="s">
         <v>622</v>
       </c>
-      <c r="R26" s="415"/>
-      <c r="S26" s="415"/>
-      <c r="T26" s="419"/>
-      <c r="U26" s="419"/>
-      <c r="V26" s="419"/>
-      <c r="W26" s="419"/>
-      <c r="X26" s="419"/>
-      <c r="Y26" s="419"/>
-      <c r="Z26" s="418" t="s">
+      <c r="R26" s="425"/>
+      <c r="S26" s="425"/>
+      <c r="T26" s="424"/>
+      <c r="U26" s="424"/>
+      <c r="V26" s="424"/>
+      <c r="W26" s="424"/>
+      <c r="X26" s="424"/>
+      <c r="Y26" s="424"/>
+      <c r="Z26" s="423" t="s">
         <v>674</v>
       </c>
-      <c r="AA26" s="418"/>
-      <c r="AB26" s="419"/>
-      <c r="AC26" s="419"/>
-      <c r="AD26" s="419"/>
-      <c r="AE26" s="419"/>
-      <c r="AF26" s="418" t="s">
+      <c r="AA26" s="423"/>
+      <c r="AB26" s="424"/>
+      <c r="AC26" s="424"/>
+      <c r="AD26" s="424"/>
+      <c r="AE26" s="424"/>
+      <c r="AF26" s="423" t="s">
         <v>675</v>
       </c>
-      <c r="AG26" s="418"/>
-      <c r="AH26" s="418" t="s">
+      <c r="AG26" s="423"/>
+      <c r="AH26" s="423" t="s">
         <v>676</v>
       </c>
-      <c r="AI26" s="418"/>
-      <c r="AJ26" s="419"/>
-      <c r="AK26" s="419"/>
-      <c r="AL26" s="415"/>
-      <c r="AM26" s="415"/>
-      <c r="AN26" s="417"/>
-      <c r="AO26" s="417"/>
+      <c r="AI26" s="423"/>
+      <c r="AJ26" s="424"/>
+      <c r="AK26" s="424"/>
+      <c r="AL26" s="425"/>
+      <c r="AM26" s="425"/>
+      <c r="AN26" s="428"/>
+      <c r="AO26" s="428"/>
     </row>
     <row r="27" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P27" s="423"/>
+      <c r="P27" s="421"/>
       <c r="Q27" s="413" t="s">
         <v>629</v>
       </c>
-      <c r="R27" s="415"/>
-      <c r="S27" s="415"/>
-      <c r="T27" s="419"/>
-      <c r="U27" s="419"/>
-      <c r="V27" s="419"/>
-      <c r="W27" s="419"/>
-      <c r="X27" s="419"/>
-      <c r="Y27" s="419"/>
-      <c r="Z27" s="418" t="s">
+      <c r="R27" s="425"/>
+      <c r="S27" s="425"/>
+      <c r="T27" s="424"/>
+      <c r="U27" s="424"/>
+      <c r="V27" s="424"/>
+      <c r="W27" s="424"/>
+      <c r="X27" s="424"/>
+      <c r="Y27" s="424"/>
+      <c r="Z27" s="423" t="s">
         <v>677</v>
       </c>
-      <c r="AA27" s="418"/>
-      <c r="AB27" s="419"/>
-      <c r="AC27" s="419"/>
-      <c r="AD27" s="419"/>
-      <c r="AE27" s="419"/>
-      <c r="AF27" s="419"/>
-      <c r="AG27" s="419"/>
-      <c r="AH27" s="419"/>
-      <c r="AI27" s="419"/>
-      <c r="AJ27" s="419"/>
-      <c r="AK27" s="419"/>
-      <c r="AL27" s="415"/>
-      <c r="AM27" s="415"/>
-      <c r="AN27" s="417"/>
-      <c r="AO27" s="417"/>
+      <c r="AA27" s="423"/>
+      <c r="AB27" s="424"/>
+      <c r="AC27" s="424"/>
+      <c r="AD27" s="424"/>
+      <c r="AE27" s="424"/>
+      <c r="AF27" s="424"/>
+      <c r="AG27" s="424"/>
+      <c r="AH27" s="424"/>
+      <c r="AI27" s="424"/>
+      <c r="AJ27" s="424"/>
+      <c r="AK27" s="424"/>
+      <c r="AL27" s="425"/>
+      <c r="AM27" s="425"/>
+      <c r="AN27" s="428"/>
+      <c r="AO27" s="428"/>
     </row>
     <row r="28" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P28" s="423" t="s">
+      <c r="P28" s="421" t="s">
         <v>678</v>
       </c>
       <c r="Q28" s="412" t="s">
         <v>679</v>
       </c>
-      <c r="R28" s="418" t="s">
+      <c r="R28" s="423" t="s">
         <v>680</v>
       </c>
-      <c r="S28" s="418"/>
-      <c r="T28" s="419"/>
-      <c r="U28" s="419"/>
-      <c r="V28" s="419"/>
-      <c r="W28" s="419"/>
-      <c r="X28" s="418" t="s">
+      <c r="S28" s="423"/>
+      <c r="T28" s="424"/>
+      <c r="U28" s="424"/>
+      <c r="V28" s="424"/>
+      <c r="W28" s="424"/>
+      <c r="X28" s="423" t="s">
         <v>681</v>
       </c>
-      <c r="Y28" s="418"/>
-      <c r="Z28" s="418" t="s">
+      <c r="Y28" s="423"/>
+      <c r="Z28" s="423" t="s">
         <v>682</v>
       </c>
-      <c r="AA28" s="418"/>
-      <c r="AB28" s="419"/>
-      <c r="AC28" s="419"/>
-      <c r="AD28" s="419"/>
-      <c r="AE28" s="419"/>
-      <c r="AF28" s="418" t="s">
+      <c r="AA28" s="423"/>
+      <c r="AB28" s="424"/>
+      <c r="AC28" s="424"/>
+      <c r="AD28" s="424"/>
+      <c r="AE28" s="424"/>
+      <c r="AF28" s="423" t="s">
         <v>683</v>
       </c>
-      <c r="AG28" s="418"/>
-      <c r="AH28" s="419"/>
-      <c r="AI28" s="419"/>
-      <c r="AJ28" s="419"/>
-      <c r="AK28" s="419"/>
-      <c r="AL28" s="415"/>
-      <c r="AM28" s="415"/>
-      <c r="AN28" s="417"/>
-      <c r="AO28" s="417"/>
+      <c r="AG28" s="423"/>
+      <c r="AH28" s="424"/>
+      <c r="AI28" s="424"/>
+      <c r="AJ28" s="424"/>
+      <c r="AK28" s="424"/>
+      <c r="AL28" s="425"/>
+      <c r="AM28" s="425"/>
+      <c r="AN28" s="428"/>
+      <c r="AO28" s="428"/>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P29" s="423"/>
+      <c r="P29" s="421"/>
       <c r="Q29" s="412" t="s">
         <v>684</v>
       </c>
-      <c r="R29" s="418" t="s">
+      <c r="R29" s="423" t="s">
         <v>685</v>
       </c>
-      <c r="S29" s="418"/>
-      <c r="T29" s="419"/>
-      <c r="U29" s="419"/>
-      <c r="V29" s="419"/>
-      <c r="W29" s="419"/>
-      <c r="X29" s="418" t="s">
+      <c r="S29" s="423"/>
+      <c r="T29" s="424"/>
+      <c r="U29" s="424"/>
+      <c r="V29" s="424"/>
+      <c r="W29" s="424"/>
+      <c r="X29" s="423" t="s">
         <v>686</v>
       </c>
-      <c r="Y29" s="418"/>
-      <c r="Z29" s="418" t="s">
+      <c r="Y29" s="423"/>
+      <c r="Z29" s="423" t="s">
         <v>687</v>
       </c>
-      <c r="AA29" s="418"/>
-      <c r="AB29" s="419"/>
-      <c r="AC29" s="419"/>
-      <c r="AD29" s="419"/>
-      <c r="AE29" s="419"/>
-      <c r="AF29" s="418" t="s">
+      <c r="AA29" s="423"/>
+      <c r="AB29" s="424"/>
+      <c r="AC29" s="424"/>
+      <c r="AD29" s="424"/>
+      <c r="AE29" s="424"/>
+      <c r="AF29" s="423" t="s">
         <v>688</v>
       </c>
-      <c r="AG29" s="418"/>
-      <c r="AH29" s="419"/>
-      <c r="AI29" s="419"/>
-      <c r="AJ29" s="419"/>
-      <c r="AK29" s="419"/>
-      <c r="AL29" s="415"/>
-      <c r="AM29" s="415"/>
-      <c r="AN29" s="417"/>
-      <c r="AO29" s="417"/>
+      <c r="AG29" s="423"/>
+      <c r="AH29" s="424"/>
+      <c r="AI29" s="424"/>
+      <c r="AJ29" s="424"/>
+      <c r="AK29" s="424"/>
+      <c r="AL29" s="425"/>
+      <c r="AM29" s="425"/>
+      <c r="AN29" s="428"/>
+      <c r="AO29" s="428"/>
     </row>
     <row r="30" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P30" s="423"/>
+      <c r="P30" s="421"/>
       <c r="Q30" s="412" t="s">
         <v>549</v>
       </c>
-      <c r="R30" s="418" t="s">
+      <c r="R30" s="423" t="s">
         <v>689</v>
       </c>
-      <c r="S30" s="418"/>
-      <c r="T30" s="419"/>
-      <c r="U30" s="419"/>
-      <c r="V30" s="419"/>
-      <c r="W30" s="419"/>
-      <c r="X30" s="418" t="s">
+      <c r="S30" s="423"/>
+      <c r="T30" s="424"/>
+      <c r="U30" s="424"/>
+      <c r="V30" s="424"/>
+      <c r="W30" s="424"/>
+      <c r="X30" s="423" t="s">
         <v>690</v>
       </c>
-      <c r="Y30" s="418"/>
-      <c r="Z30" s="418" t="s">
+      <c r="Y30" s="423"/>
+      <c r="Z30" s="423" t="s">
         <v>691</v>
       </c>
-      <c r="AA30" s="418"/>
-      <c r="AB30" s="419"/>
-      <c r="AC30" s="419"/>
-      <c r="AD30" s="419"/>
-      <c r="AE30" s="419"/>
-      <c r="AF30" s="418" t="s">
+      <c r="AA30" s="423"/>
+      <c r="AB30" s="424"/>
+      <c r="AC30" s="424"/>
+      <c r="AD30" s="424"/>
+      <c r="AE30" s="424"/>
+      <c r="AF30" s="423" t="s">
         <v>692</v>
       </c>
-      <c r="AG30" s="418"/>
-      <c r="AH30" s="419"/>
-      <c r="AI30" s="419"/>
-      <c r="AJ30" s="419"/>
-      <c r="AK30" s="419"/>
-      <c r="AL30" s="415"/>
-      <c r="AM30" s="415"/>
-      <c r="AN30" s="417"/>
-      <c r="AO30" s="417"/>
+      <c r="AG30" s="423"/>
+      <c r="AH30" s="424"/>
+      <c r="AI30" s="424"/>
+      <c r="AJ30" s="424"/>
+      <c r="AK30" s="424"/>
+      <c r="AL30" s="425"/>
+      <c r="AM30" s="425"/>
+      <c r="AN30" s="428"/>
+      <c r="AO30" s="428"/>
     </row>
     <row r="31" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P31" s="423"/>
+      <c r="P31" s="421"/>
       <c r="Q31" s="412" t="s">
         <v>693</v>
       </c>
-      <c r="R31" s="419"/>
-      <c r="S31" s="419"/>
-      <c r="T31" s="419"/>
-      <c r="U31" s="419"/>
-      <c r="V31" s="419"/>
-      <c r="W31" s="419"/>
-      <c r="X31" s="419"/>
-      <c r="Y31" s="419"/>
-      <c r="Z31" s="418" t="s">
+      <c r="R31" s="424"/>
+      <c r="S31" s="424"/>
+      <c r="T31" s="424"/>
+      <c r="U31" s="424"/>
+      <c r="V31" s="424"/>
+      <c r="W31" s="424"/>
+      <c r="X31" s="424"/>
+      <c r="Y31" s="424"/>
+      <c r="Z31" s="423" t="s">
         <v>694</v>
       </c>
-      <c r="AA31" s="418"/>
-      <c r="AB31" s="419"/>
-      <c r="AC31" s="419"/>
-      <c r="AD31" s="419"/>
-      <c r="AE31" s="419"/>
-      <c r="AF31" s="419"/>
-      <c r="AG31" s="419"/>
-      <c r="AH31" s="419"/>
-      <c r="AI31" s="419"/>
-      <c r="AJ31" s="419"/>
-      <c r="AK31" s="419"/>
-      <c r="AL31" s="415"/>
-      <c r="AM31" s="415"/>
-      <c r="AN31" s="417"/>
-      <c r="AO31" s="417"/>
+      <c r="AA31" s="423"/>
+      <c r="AB31" s="424"/>
+      <c r="AC31" s="424"/>
+      <c r="AD31" s="424"/>
+      <c r="AE31" s="424"/>
+      <c r="AF31" s="424"/>
+      <c r="AG31" s="424"/>
+      <c r="AH31" s="424"/>
+      <c r="AI31" s="424"/>
+      <c r="AJ31" s="424"/>
+      <c r="AK31" s="424"/>
+      <c r="AL31" s="425"/>
+      <c r="AM31" s="425"/>
+      <c r="AN31" s="428"/>
+      <c r="AO31" s="428"/>
     </row>
     <row r="32" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="P32" s="423"/>
+      <c r="P32" s="421"/>
       <c r="Q32" s="413" t="s">
         <v>695</v>
       </c>
-      <c r="R32" s="419"/>
-      <c r="S32" s="419"/>
-      <c r="T32" s="419"/>
-      <c r="U32" s="419"/>
-      <c r="V32" s="419"/>
-      <c r="W32" s="419"/>
-      <c r="X32" s="419"/>
-      <c r="Y32" s="419"/>
-      <c r="Z32" s="418" t="s">
+      <c r="R32" s="424"/>
+      <c r="S32" s="424"/>
+      <c r="T32" s="424"/>
+      <c r="U32" s="424"/>
+      <c r="V32" s="424"/>
+      <c r="W32" s="424"/>
+      <c r="X32" s="424"/>
+      <c r="Y32" s="424"/>
+      <c r="Z32" s="423" t="s">
         <v>696</v>
       </c>
-      <c r="AA32" s="418"/>
-      <c r="AB32" s="419"/>
-      <c r="AC32" s="419"/>
-      <c r="AD32" s="419"/>
-      <c r="AE32" s="419"/>
-      <c r="AF32" s="419"/>
-      <c r="AG32" s="419"/>
-      <c r="AH32" s="419"/>
-      <c r="AI32" s="419"/>
-      <c r="AJ32" s="419"/>
-      <c r="AK32" s="419"/>
-      <c r="AL32" s="415"/>
-      <c r="AM32" s="415"/>
-      <c r="AN32" s="417"/>
-      <c r="AO32" s="417"/>
+      <c r="AA32" s="423"/>
+      <c r="AB32" s="424"/>
+      <c r="AC32" s="424"/>
+      <c r="AD32" s="424"/>
+      <c r="AE32" s="424"/>
+      <c r="AF32" s="424"/>
+      <c r="AG32" s="424"/>
+      <c r="AH32" s="424"/>
+      <c r="AI32" s="424"/>
+      <c r="AJ32" s="424"/>
+      <c r="AK32" s="424"/>
+      <c r="AL32" s="425"/>
+      <c r="AM32" s="425"/>
+      <c r="AN32" s="428"/>
+      <c r="AO32" s="428"/>
     </row>
     <row r="33" spans="16:41" x14ac:dyDescent="0.2">
-      <c r="P33" s="423" t="s">
+      <c r="P33" s="421" t="s">
         <v>697</v>
       </c>
       <c r="Q33" s="413" t="s">
         <v>684</v>
       </c>
-      <c r="R33" s="418" t="s">
+      <c r="R33" s="423" t="s">
         <v>698</v>
       </c>
-      <c r="S33" s="418"/>
-      <c r="T33" s="419"/>
-      <c r="U33" s="419"/>
-      <c r="V33" s="419"/>
-      <c r="W33" s="419"/>
-      <c r="X33" s="419"/>
-      <c r="Y33" s="419"/>
-      <c r="Z33" s="418" t="s">
+      <c r="S33" s="423"/>
+      <c r="T33" s="424"/>
+      <c r="U33" s="424"/>
+      <c r="V33" s="424"/>
+      <c r="W33" s="424"/>
+      <c r="X33" s="424"/>
+      <c r="Y33" s="424"/>
+      <c r="Z33" s="423" t="s">
         <v>699</v>
       </c>
-      <c r="AA33" s="418"/>
-      <c r="AB33" s="419"/>
-      <c r="AC33" s="419"/>
-      <c r="AD33" s="418" t="s">
+      <c r="AA33" s="423"/>
+      <c r="AB33" s="424"/>
+      <c r="AC33" s="424"/>
+      <c r="AD33" s="423" t="s">
         <v>700</v>
       </c>
-      <c r="AE33" s="418"/>
-      <c r="AF33" s="418" t="s">
+      <c r="AE33" s="423"/>
+      <c r="AF33" s="423" t="s">
         <v>701</v>
       </c>
-      <c r="AG33" s="418"/>
-      <c r="AH33" s="418" t="s">
+      <c r="AG33" s="423"/>
+      <c r="AH33" s="423" t="s">
         <v>702</v>
       </c>
-      <c r="AI33" s="418"/>
-      <c r="AJ33" s="418" t="s">
+      <c r="AI33" s="423"/>
+      <c r="AJ33" s="423" t="s">
         <v>703</v>
       </c>
-      <c r="AK33" s="418"/>
-      <c r="AL33" s="415"/>
-      <c r="AM33" s="415"/>
-      <c r="AN33" s="417"/>
-      <c r="AO33" s="417"/>
+      <c r="AK33" s="423"/>
+      <c r="AL33" s="425"/>
+      <c r="AM33" s="425"/>
+      <c r="AN33" s="428"/>
+      <c r="AO33" s="428"/>
     </row>
     <row r="34" spans="16:41" x14ac:dyDescent="0.2">
-      <c r="P34" s="423"/>
+      <c r="P34" s="421"/>
       <c r="Q34" s="412" t="s">
         <v>704</v>
       </c>
-      <c r="R34" s="418" t="s">
+      <c r="R34" s="423" t="s">
         <v>705</v>
       </c>
-      <c r="S34" s="418"/>
-      <c r="T34" s="419"/>
-      <c r="U34" s="419"/>
-      <c r="V34" s="419"/>
-      <c r="W34" s="419"/>
-      <c r="X34" s="419"/>
-      <c r="Y34" s="419"/>
-      <c r="Z34" s="418" t="s">
+      <c r="S34" s="423"/>
+      <c r="T34" s="424"/>
+      <c r="U34" s="424"/>
+      <c r="V34" s="424"/>
+      <c r="W34" s="424"/>
+      <c r="X34" s="424"/>
+      <c r="Y34" s="424"/>
+      <c r="Z34" s="423" t="s">
         <v>706</v>
       </c>
-      <c r="AA34" s="418"/>
-      <c r="AB34" s="419"/>
-      <c r="AC34" s="419"/>
-      <c r="AD34" s="418" t="s">
+      <c r="AA34" s="423"/>
+      <c r="AB34" s="424"/>
+      <c r="AC34" s="424"/>
+      <c r="AD34" s="423" t="s">
         <v>707</v>
       </c>
-      <c r="AE34" s="418"/>
-      <c r="AF34" s="418" t="s">
+      <c r="AE34" s="423"/>
+      <c r="AF34" s="423" t="s">
         <v>708</v>
       </c>
-      <c r="AG34" s="418"/>
-      <c r="AH34" s="418" t="s">
+      <c r="AG34" s="423"/>
+      <c r="AH34" s="423" t="s">
         <v>709</v>
       </c>
-      <c r="AI34" s="418"/>
-      <c r="AJ34" s="418" t="s">
+      <c r="AI34" s="423"/>
+      <c r="AJ34" s="423" t="s">
         <v>710</v>
       </c>
-      <c r="AK34" s="418"/>
-      <c r="AL34" s="415"/>
-      <c r="AM34" s="415"/>
-      <c r="AN34" s="416"/>
-      <c r="AO34" s="416"/>
+      <c r="AK34" s="423"/>
+      <c r="AL34" s="425"/>
+      <c r="AM34" s="425"/>
+      <c r="AN34" s="427"/>
+      <c r="AO34" s="427"/>
     </row>
   </sheetData>
   <mergeCells count="183">
-    <mergeCell ref="C2:AO2"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="W4:AF4"/>
-    <mergeCell ref="AG4:AK4"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="AL33:AM33"/>
+    <mergeCell ref="AL34:AM34"/>
+    <mergeCell ref="AN23:AO23"/>
+    <mergeCell ref="AN24:AO24"/>
+    <mergeCell ref="AN25:AO25"/>
+    <mergeCell ref="AN26:AO26"/>
+    <mergeCell ref="AN27:AO27"/>
+    <mergeCell ref="AN28:AO28"/>
+    <mergeCell ref="AN29:AO29"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AN31:AO31"/>
+    <mergeCell ref="AN32:AO32"/>
+    <mergeCell ref="AN33:AO33"/>
+    <mergeCell ref="AN34:AO34"/>
+    <mergeCell ref="AL28:AM28"/>
+    <mergeCell ref="AL29:AM29"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AL31:AM31"/>
+    <mergeCell ref="AL32:AM32"/>
+    <mergeCell ref="AL23:AM23"/>
+    <mergeCell ref="AL24:AM24"/>
+    <mergeCell ref="AL25:AM25"/>
+    <mergeCell ref="AL26:AM26"/>
+    <mergeCell ref="AL27:AM27"/>
+    <mergeCell ref="AH33:AI33"/>
+    <mergeCell ref="AH34:AI34"/>
+    <mergeCell ref="AJ23:AK23"/>
+    <mergeCell ref="AJ24:AK24"/>
+    <mergeCell ref="AJ25:AK25"/>
+    <mergeCell ref="AJ26:AK26"/>
+    <mergeCell ref="AJ27:AK27"/>
+    <mergeCell ref="AJ28:AK28"/>
+    <mergeCell ref="AJ29:AK29"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AJ31:AK31"/>
+    <mergeCell ref="AJ32:AK32"/>
+    <mergeCell ref="AJ33:AK33"/>
+    <mergeCell ref="AJ34:AK34"/>
+    <mergeCell ref="AH28:AI28"/>
+    <mergeCell ref="AH29:AI29"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AH31:AI31"/>
+    <mergeCell ref="AH32:AI32"/>
+    <mergeCell ref="AH23:AI23"/>
+    <mergeCell ref="AH24:AI24"/>
+    <mergeCell ref="AH25:AI25"/>
+    <mergeCell ref="AH26:AI26"/>
+    <mergeCell ref="AH27:AI27"/>
+    <mergeCell ref="AD31:AE31"/>
+    <mergeCell ref="AD32:AE32"/>
+    <mergeCell ref="AD33:AE33"/>
+    <mergeCell ref="AD34:AE34"/>
+    <mergeCell ref="AF23:AG23"/>
+    <mergeCell ref="AF24:AG24"/>
+    <mergeCell ref="AF25:AG25"/>
+    <mergeCell ref="AF26:AG26"/>
+    <mergeCell ref="AF27:AG27"/>
+    <mergeCell ref="AF28:AG28"/>
+    <mergeCell ref="AF29:AG29"/>
+    <mergeCell ref="AF30:AG30"/>
+    <mergeCell ref="AF31:AG31"/>
+    <mergeCell ref="AF32:AG32"/>
+    <mergeCell ref="AF33:AG33"/>
+    <mergeCell ref="AF34:AG34"/>
+    <mergeCell ref="AD26:AE26"/>
+    <mergeCell ref="AD27:AE27"/>
+    <mergeCell ref="AD28:AE28"/>
+    <mergeCell ref="AD29:AE29"/>
+    <mergeCell ref="AD30:AE30"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="AD23:AE23"/>
+    <mergeCell ref="AD24:AE24"/>
+    <mergeCell ref="AD25:AE25"/>
+    <mergeCell ref="AB33:AC33"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="AB28:AC28"/>
+    <mergeCell ref="AB29:AC29"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AB32:AC32"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="AB24:AC24"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="AB27:AC27"/>
+    <mergeCell ref="X33:Y33"/>
+    <mergeCell ref="X34:Y34"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="Z27:AA27"/>
+    <mergeCell ref="Z28:AA28"/>
+    <mergeCell ref="Z29:AA29"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="Z31:AA31"/>
+    <mergeCell ref="Z32:AA32"/>
+    <mergeCell ref="Z33:AA33"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="X29:Y29"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="X32:Y32"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AL22:AM22"/>
+    <mergeCell ref="AN22:AO22"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="AB25:AC25"/>
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="W21:AF21"/>
     <mergeCell ref="P23:P27"/>
@@ -13252,169 +13540,48 @@
     <mergeCell ref="AD22:AE22"/>
     <mergeCell ref="AF22:AG22"/>
     <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AL22:AM22"/>
-    <mergeCell ref="AN22:AO22"/>
-    <mergeCell ref="X25:Y25"/>
-    <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V34:W34"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="AB27:AC27"/>
-    <mergeCell ref="X33:Y33"/>
-    <mergeCell ref="X34:Y34"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z26:AA26"/>
-    <mergeCell ref="Z27:AA27"/>
-    <mergeCell ref="Z28:AA28"/>
-    <mergeCell ref="Z29:AA29"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="Z31:AA31"/>
-    <mergeCell ref="Z32:AA32"/>
-    <mergeCell ref="Z33:AA33"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="X29:Y29"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="X32:Y32"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="AD23:AE23"/>
-    <mergeCell ref="AD24:AE24"/>
-    <mergeCell ref="AD25:AE25"/>
-    <mergeCell ref="AB33:AC33"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="R32:S32"/>
-    <mergeCell ref="R33:S33"/>
-    <mergeCell ref="R34:S34"/>
-    <mergeCell ref="AB28:AC28"/>
-    <mergeCell ref="AB29:AC29"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AB32:AC32"/>
-    <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="AB24:AC24"/>
-    <mergeCell ref="AD31:AE31"/>
-    <mergeCell ref="AD32:AE32"/>
-    <mergeCell ref="AD33:AE33"/>
-    <mergeCell ref="AD34:AE34"/>
-    <mergeCell ref="AF23:AG23"/>
-    <mergeCell ref="AF24:AG24"/>
-    <mergeCell ref="AF25:AG25"/>
-    <mergeCell ref="AF26:AG26"/>
-    <mergeCell ref="AF27:AG27"/>
-    <mergeCell ref="AF28:AG28"/>
-    <mergeCell ref="AF29:AG29"/>
-    <mergeCell ref="AF30:AG30"/>
-    <mergeCell ref="AF31:AG31"/>
-    <mergeCell ref="AF32:AG32"/>
-    <mergeCell ref="AF33:AG33"/>
-    <mergeCell ref="AF34:AG34"/>
-    <mergeCell ref="AD26:AE26"/>
-    <mergeCell ref="AD27:AE27"/>
-    <mergeCell ref="AD28:AE28"/>
-    <mergeCell ref="AD29:AE29"/>
-    <mergeCell ref="AD30:AE30"/>
-    <mergeCell ref="AH33:AI33"/>
-    <mergeCell ref="AH34:AI34"/>
-    <mergeCell ref="AJ23:AK23"/>
-    <mergeCell ref="AJ24:AK24"/>
-    <mergeCell ref="AJ25:AK25"/>
-    <mergeCell ref="AJ26:AK26"/>
-    <mergeCell ref="AJ27:AK27"/>
-    <mergeCell ref="AJ28:AK28"/>
-    <mergeCell ref="AJ29:AK29"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AJ31:AK31"/>
-    <mergeCell ref="AJ32:AK32"/>
-    <mergeCell ref="AJ33:AK33"/>
-    <mergeCell ref="AJ34:AK34"/>
-    <mergeCell ref="AH28:AI28"/>
-    <mergeCell ref="AH29:AI29"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AH31:AI31"/>
-    <mergeCell ref="AH32:AI32"/>
-    <mergeCell ref="AH23:AI23"/>
-    <mergeCell ref="AH24:AI24"/>
-    <mergeCell ref="AH25:AI25"/>
-    <mergeCell ref="AH26:AI26"/>
-    <mergeCell ref="AH27:AI27"/>
-    <mergeCell ref="AL33:AM33"/>
-    <mergeCell ref="AL34:AM34"/>
-    <mergeCell ref="AN23:AO23"/>
-    <mergeCell ref="AN24:AO24"/>
-    <mergeCell ref="AN25:AO25"/>
-    <mergeCell ref="AN26:AO26"/>
-    <mergeCell ref="AN27:AO27"/>
-    <mergeCell ref="AN28:AO28"/>
-    <mergeCell ref="AN29:AO29"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AN31:AO31"/>
-    <mergeCell ref="AN32:AO32"/>
-    <mergeCell ref="AN33:AO33"/>
-    <mergeCell ref="AN34:AO34"/>
-    <mergeCell ref="AL28:AM28"/>
-    <mergeCell ref="AL29:AM29"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AL31:AM31"/>
-    <mergeCell ref="AL32:AM32"/>
-    <mergeCell ref="AL23:AM23"/>
-    <mergeCell ref="AL24:AM24"/>
-    <mergeCell ref="AL25:AM25"/>
-    <mergeCell ref="AL26:AM26"/>
-    <mergeCell ref="AL27:AM27"/>
+    <mergeCell ref="C2:AO2"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="W4:AF4"/>
+    <mergeCell ref="AG4:AK4"/>
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <conditionalFormatting sqref="R6:AO18">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(R6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:L12">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(C6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23:AO34">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="9">
       <formula>LEN(TRIM(R23))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR9">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(AR9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS9">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(AS9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13424,10 +13591,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416F08AC-9E91-274B-B0C5-FBF01BD4A382}">
-  <dimension ref="B3:AG49"/>
+  <dimension ref="B3:AG48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A178" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13455,7 +13622,7 @@
       <c r="B4" t="s">
         <v>711</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>735</v>
       </c>
       <c r="U4" s="32"/>
@@ -13476,6 +13643,9 @@
       <c r="B5" t="s">
         <v>549</v>
       </c>
+      <c r="C5" t="s">
+        <v>712</v>
+      </c>
       <c r="F5" t="s">
         <v>736</v>
       </c>
@@ -13500,9 +13670,6 @@
       <c r="AG5" s="32"/>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>712</v>
-      </c>
       <c r="F6" t="s">
         <v>738</v>
       </c>
@@ -13584,6 +13751,9 @@
       <c r="B8" t="s">
         <v>713</v>
       </c>
+      <c r="C8" t="s">
+        <v>714</v>
+      </c>
       <c r="F8" s="309" t="s">
         <v>742</v>
       </c>
@@ -13626,9 +13796,6 @@
       <c r="AG8" s="32"/>
     </row>
     <row r="9" spans="2:33" ht="19" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>714</v>
-      </c>
       <c r="E9" s="311"/>
       <c r="F9" s="97" t="s">
         <v>744</v>
@@ -13718,6 +13885,9 @@
       <c r="B11" t="s">
         <v>715</v>
       </c>
+      <c r="C11" t="s">
+        <v>716</v>
+      </c>
       <c r="E11" s="311"/>
       <c r="F11" s="97" t="s">
         <v>748</v>
@@ -13764,6 +13934,9 @@
       <c r="B12" t="s">
         <v>556</v>
       </c>
+      <c r="C12" t="s">
+        <v>717</v>
+      </c>
       <c r="E12" s="311"/>
       <c r="F12" s="97" t="s">
         <v>750</v>
@@ -13807,9 +13980,6 @@
       <c r="AG12" s="32"/>
     </row>
     <row r="13" spans="2:33" ht="19" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>716</v>
-      </c>
       <c r="E13" s="311"/>
       <c r="F13" s="309" t="s">
         <v>752</v>
@@ -13853,9 +14023,6 @@
       <c r="AG13" s="32"/>
     </row>
     <row r="14" spans="2:33" ht="19" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>717</v>
-      </c>
       <c r="E14" s="311"/>
       <c r="F14" s="97"/>
       <c r="G14" s="97"/>
@@ -13895,8 +14062,7 @@
       <c r="AG14" s="32"/>
     </row>
     <row r="15" spans="2:33" ht="19" x14ac:dyDescent="0.25">
-      <c r="E15" s="311"/>
-      <c r="F15" s="97" t="s">
+      <c r="E15" s="97" t="s">
         <v>754</v>
       </c>
       <c r="G15" s="97"/>
@@ -13939,6 +14105,9 @@
       <c r="B16" t="s">
         <v>713</v>
       </c>
+      <c r="C16" t="s">
+        <v>718</v>
+      </c>
       <c r="E16" s="311"/>
       <c r="F16" s="97" t="s">
         <v>755</v>
@@ -13984,8 +14153,8 @@
       <c r="AG16" s="32"/>
     </row>
     <row r="17" spans="2:33" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>718</v>
+      <c r="C17" t="s">
+        <v>719</v>
       </c>
       <c r="E17" s="311"/>
       <c r="F17" s="97" t="s">
@@ -14032,9 +14201,6 @@
       <c r="AG17" s="32"/>
     </row>
     <row r="18" spans="2:33" ht="19" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>719</v>
-      </c>
       <c r="E18" s="311"/>
       <c r="F18" s="309" t="s">
         <v>761</v>
@@ -14106,6 +14272,9 @@
       <c r="B20" t="s">
         <v>715</v>
       </c>
+      <c r="C20" t="s">
+        <v>720</v>
+      </c>
       <c r="E20" s="312"/>
       <c r="F20" s="97" t="s">
         <v>767</v>
@@ -14118,9 +14287,6 @@
       </c>
       <c r="I20" s="310"/>
       <c r="J20" s="97"/>
-      <c r="K20" s="310"/>
-      <c r="L20" s="97"/>
-      <c r="M20" s="97"/>
       <c r="N20" s="97"/>
       <c r="O20" s="97"/>
       <c r="P20" s="310"/>
@@ -14139,9 +14305,6 @@
       <c r="AG20" s="32"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>720</v>
-      </c>
       <c r="E21" s="97"/>
       <c r="F21" t="s">
         <v>770</v>
@@ -14171,6 +14334,9 @@
       <c r="G22" t="s">
         <v>773</v>
       </c>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
       <c r="U22" s="32"/>
       <c r="V22" s="32"/>
       <c r="W22" s="32"/>
@@ -14185,11 +14351,17 @@
       <c r="AF22" s="32"/>
       <c r="AG22" s="32"/>
     </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:33" ht="19" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>721</v>
       </c>
+      <c r="C23" t="s">
+        <v>722</v>
+      </c>
       <c r="E23" s="97"/>
+      <c r="K23" s="310"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
       <c r="U23" s="32"/>
       <c r="V23" s="32"/>
       <c r="W23" s="32"/>
@@ -14204,13 +14376,16 @@
       <c r="AF23" s="32"/>
       <c r="AG23" s="32"/>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:33" ht="19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>664</v>
       </c>
-      <c r="F24" t="s">
+      <c r="E24" t="s">
         <v>774</v>
       </c>
+      <c r="K24" s="97"/>
+      <c r="L24" s="310"/>
+      <c r="M24" s="97"/>
       <c r="U24" s="32"/>
       <c r="V24" s="32"/>
       <c r="W24" s="32"/>
@@ -14226,9 +14401,6 @@
       <c r="AG24" s="32"/>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>722</v>
-      </c>
       <c r="F25" t="s">
         <v>775</v>
       </c>
@@ -14238,6 +14410,9 @@
       <c r="H25" t="s">
         <v>777</v>
       </c>
+      <c r="K25" s="97"/>
+      <c r="L25" s="97"/>
+      <c r="M25" s="97"/>
       <c r="U25" s="32"/>
       <c r="V25" s="32"/>
       <c r="W25" s="32"/>
@@ -14252,7 +14427,7 @@
       <c r="AF25" s="32"/>
       <c r="AG25" s="32"/>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:33" ht="19" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>778</v>
       </c>
@@ -14262,6 +14437,9 @@
       <c r="H26" t="s">
         <v>780</v>
       </c>
+      <c r="K26" s="310"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="310"/>
       <c r="U26" s="32"/>
       <c r="V26" s="32"/>
       <c r="W26" s="32"/>
@@ -14276,7 +14454,7 @@
       <c r="AF26" s="32"/>
       <c r="AG26" s="32"/>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:33" ht="19" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>723</v>
       </c>
@@ -14289,8 +14467,11 @@
       <c r="H27" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="K27" s="310"/>
+      <c r="L27" s="310"/>
+      <c r="M27" s="310"/>
+    </row>
+    <row r="28" spans="2:33" ht="19" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>784</v>
       </c>
@@ -14300,11 +14481,17 @@
       <c r="H28" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="K28" s="310"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="310"/>
+    </row>
+    <row r="29" spans="2:33" ht="19" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>600</v>
       </c>
+      <c r="C29" t="s">
+        <v>724</v>
+      </c>
       <c r="F29" t="s">
         <v>787</v>
       </c>
@@ -14314,10 +14501,13 @@
       <c r="H29" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>724</v>
+      <c r="K29" s="310"/>
+      <c r="L29" s="97"/>
+      <c r="M29" s="310"/>
+    </row>
+    <row r="30" spans="2:33" ht="19" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>725</v>
       </c>
       <c r="F30" t="s">
         <v>790</v>
@@ -14328,11 +14518,11 @@
       <c r="H30" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>725</v>
-      </c>
+      <c r="K30" s="310"/>
+      <c r="L30" s="97"/>
+      <c r="M30" s="310"/>
+    </row>
+    <row r="31" spans="2:33" ht="19" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>793</v>
       </c>
@@ -14342,8 +14532,11 @@
       <c r="H31" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="K31" s="310"/>
+      <c r="L31" s="310"/>
+      <c r="M31" s="310"/>
+    </row>
+    <row r="32" spans="2:33" ht="19" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>796</v>
       </c>
@@ -14353,11 +14546,15 @@
       <c r="H32" t="s">
         <v>798</v>
       </c>
+      <c r="M32" s="310"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>726</v>
       </c>
+      <c r="C33" t="s">
+        <v>727</v>
+      </c>
       <c r="F33" t="s">
         <v>799</v>
       </c>
@@ -14366,8 +14563,8 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>727</v>
+      <c r="C34" t="s">
+        <v>728</v>
       </c>
       <c r="F34" t="s">
         <v>801</v>
@@ -14376,13 +14573,8 @@
         <v>802</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>728</v>
-      </c>
-    </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F36" t="s">
+      <c r="E36" t="s">
         <v>803</v>
       </c>
     </row>
@@ -14390,6 +14582,9 @@
       <c r="B37" t="s">
         <v>715</v>
       </c>
+      <c r="C37" t="s">
+        <v>729</v>
+      </c>
       <c r="F37" t="s">
         <v>804</v>
       </c>
@@ -14409,9 +14604,6 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>729</v>
-      </c>
       <c r="F39" t="s">
         <v>808</v>
       </c>
@@ -14431,6 +14623,9 @@
       <c r="B41" t="s">
         <v>730</v>
       </c>
+      <c r="C41" t="s">
+        <v>732</v>
+      </c>
       <c r="F41" t="s">
         <v>812</v>
       </c>
@@ -14443,18 +14638,11 @@
         <v>731</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>732</v>
-      </c>
-    </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+      <c r="C45" t="s">
         <v>733</v>
       </c>
     </row>
@@ -14462,9 +14650,7 @@
       <c r="B48" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+      <c r="C48" t="s">
         <v>734</v>
       </c>
     </row>
@@ -14477,7 +14663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DA89D9-1C1E-6540-BE07-11234B4F16D9}">
   <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F22" sqref="F22:F111"/>
     </sheetView>
@@ -14486,7 +14672,7 @@
   <cols>
     <col min="1" max="1" width="5.1640625" style="83" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="92" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="440" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="415" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="83" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="83" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" style="83" bestFit="1" customWidth="1"/>
@@ -14501,7 +14687,7 @@
       <c r="B1" s="92" t="s">
         <v>442</v>
       </c>
-      <c r="C1" s="440" t="s">
+      <c r="C1" s="415" t="s">
         <v>459</v>
       </c>
       <c r="D1" s="93" t="s">
@@ -14557,502 +14743,502 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C2" s="441" t="s">
+      <c r="C2" s="416" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C3" s="441" t="s">
+      <c r="C3" s="416" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C4" s="441" t="s">
+      <c r="C4" s="416" t="s">
         <v>895</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C5" s="441" t="s">
+      <c r="C5" s="416" t="s">
         <v>896</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C6" s="441" t="s">
+      <c r="C6" s="416" t="s">
         <v>897</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C7" s="441" t="s">
+      <c r="C7" s="416" t="s">
         <v>898</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C8" s="441" t="s">
+      <c r="C8" s="416" t="s">
         <v>899</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C9" s="441" t="s">
+      <c r="C9" s="416" t="s">
         <v>900</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C10" s="441" t="s">
+      <c r="C10" s="416" t="s">
         <v>901</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C11" s="441" t="s">
+      <c r="C11" s="416" t="s">
         <v>902</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C12" s="441" t="s">
+      <c r="C12" s="416" t="s">
         <v>903</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C13" s="441" t="s">
+      <c r="C13" s="416" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C14" s="441" t="s">
+      <c r="C14" s="416" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C15" s="441" t="s">
+      <c r="C15" s="416" t="s">
         <v>906</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C16" s="441" t="s">
+      <c r="C16" s="416" t="s">
         <v>907</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="441" t="s">
+      <c r="C17" s="416" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" s="441" t="s">
+      <c r="C18" s="416" t="s">
         <v>909</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" s="441" t="s">
+      <c r="C19" s="416" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="441" t="s">
+      <c r="C20" s="416" t="s">
         <v>911</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="441" t="s">
+      <c r="C21" s="416" t="s">
         <v>912</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="441" t="s">
+      <c r="C22" s="416" t="s">
         <v>913</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C23" s="441" t="s">
+      <c r="C23" s="416" t="s">
         <v>914</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="441" t="s">
+      <c r="C24" s="416" t="s">
         <v>915</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="441" t="s">
+      <c r="C25" s="416" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="441" t="s">
+      <c r="C26" s="416" t="s">
         <v>917</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="441" t="s">
+      <c r="C27" s="416" t="s">
         <v>918</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="441" t="s">
+      <c r="C28" s="416" t="s">
         <v>919</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C29" s="441" t="s">
+      <c r="C29" s="416" t="s">
         <v>920</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C30" s="441" t="s">
+      <c r="C30" s="416" t="s">
         <v>921</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C31" s="441" t="s">
+      <c r="C31" s="416" t="s">
         <v>922</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C32" s="441" t="s">
+      <c r="C32" s="416" t="s">
         <v>923</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="441" t="s">
+      <c r="C33" s="416" t="s">
         <v>924</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="441" t="s">
+      <c r="C34" s="416" t="s">
         <v>925</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="441" t="s">
+      <c r="C35" s="416" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="441" t="s">
+      <c r="C36" s="416" t="s">
         <v>927</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="441" t="s">
+      <c r="C37" s="416" t="s">
         <v>928</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="441" t="s">
+      <c r="C38" s="416" t="s">
         <v>929</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="441" t="s">
+      <c r="C39" s="416" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="441" t="s">
+      <c r="C40" s="416" t="s">
         <v>931</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="441" t="s">
+      <c r="C41" s="416" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="441" t="s">
+      <c r="C42" s="416" t="s">
         <v>933</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="441" t="s">
+      <c r="C43" s="416" t="s">
         <v>934</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C44" s="441" t="s">
+      <c r="C44" s="416" t="s">
         <v>935</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C45" s="441" t="s">
+      <c r="C45" s="416" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C46" s="441" t="s">
+      <c r="C46" s="416" t="s">
         <v>937</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C47" s="441" t="s">
+      <c r="C47" s="416" t="s">
         <v>938</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C48" s="441" t="s">
+      <c r="C48" s="416" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" s="441" t="s">
+      <c r="C49" s="416" t="s">
         <v>940</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C50" s="441" t="s">
+      <c r="C50" s="416" t="s">
         <v>941</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C51" s="441" t="s">
+      <c r="C51" s="416" t="s">
         <v>942</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52" s="441" t="s">
+      <c r="C52" s="416" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C53" s="441" t="s">
+      <c r="C53" s="416" t="s">
         <v>944</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C54" s="441" t="s">
+      <c r="C54" s="416" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C55" s="441" t="s">
+      <c r="C55" s="416" t="s">
         <v>946</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C56" s="441" t="s">
+      <c r="C56" s="416" t="s">
         <v>947</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C57" s="441" t="s">
+      <c r="C57" s="416" t="s">
         <v>948</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C58" s="441" t="s">
+      <c r="C58" s="416" t="s">
         <v>949</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C59" s="441" t="s">
+      <c r="C59" s="416" t="s">
         <v>950</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C60" s="441" t="s">
+      <c r="C60" s="416" t="s">
         <v>951</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C61" s="441" t="s">
+      <c r="C61" s="416" t="s">
         <v>952</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C62" s="441" t="s">
+      <c r="C62" s="416" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C63" s="441" t="s">
+      <c r="C63" s="416" t="s">
         <v>954</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C64" s="441" t="s">
+      <c r="C64" s="416" t="s">
         <v>955</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" s="441" t="s">
+      <c r="C65" s="416" t="s">
         <v>956</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66" s="441" t="s">
+      <c r="C66" s="416" t="s">
         <v>957</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C67" s="441" t="s">
+      <c r="C67" s="416" t="s">
         <v>958</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C68" s="441" t="s">
+      <c r="C68" s="416" t="s">
         <v>959</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C69" s="441" t="s">
+      <c r="C69" s="416" t="s">
         <v>960</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C70" s="441" t="s">
+      <c r="C70" s="416" t="s">
         <v>961</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C71" s="441" t="s">
+      <c r="C71" s="416" t="s">
         <v>962</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C72" s="441" t="s">
+      <c r="C72" s="416" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C73" s="441" t="s">
+      <c r="C73" s="416" t="s">
         <v>964</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C74" s="441" t="s">
+      <c r="C74" s="416" t="s">
         <v>965</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C75" s="441" t="s">
+      <c r="C75" s="416" t="s">
         <v>966</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C76" s="441" t="s">
+      <c r="C76" s="416" t="s">
         <v>967</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C77" s="441" t="s">
+      <c r="C77" s="416" t="s">
         <v>968</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C78" s="441" t="s">
+      <c r="C78" s="416" t="s">
         <v>969</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C79" s="441" t="s">
+      <c r="C79" s="416" t="s">
         <v>970</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C80" s="441" t="s">
+      <c r="C80" s="416" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C81" s="441" t="s">
+      <c r="C81" s="416" t="s">
         <v>972</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" s="441" t="s">
+      <c r="C82" s="416" t="s">
         <v>973</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C83" s="441" t="s">
+      <c r="C83" s="416" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C84" s="441" t="s">
+      <c r="C84" s="416" t="s">
         <v>975</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C85" s="441" t="s">
+      <c r="C85" s="416" t="s">
         <v>976</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C86" s="441" t="s">
+      <c r="C86" s="416" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C87" s="441" t="s">
+      <c r="C87" s="416" t="s">
         <v>978</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C88" s="441" t="s">
+      <c r="C88" s="416" t="s">
         <v>979</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C89" s="441" t="s">
+      <c r="C89" s="416" t="s">
         <v>980</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C90" s="441" t="s">
+      <c r="C90" s="416" t="s">
         <v>981</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C91" s="441" t="s">
+      <c r="C91" s="416" t="s">
         <v>982</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C92" s="441" t="s">
+      <c r="C92" s="416" t="s">
         <v>983</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C93" s="441" t="s">
+      <c r="C93" s="416" t="s">
         <v>984</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C94" s="441" t="s">
+      <c r="C94" s="416" t="s">
         <v>985</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C95" s="441" t="s">
+      <c r="C95" s="416" t="s">
         <v>986</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C96" s="441" t="s">
+      <c r="C96" s="416" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C97" s="441" t="s">
+      <c r="C97" s="416" t="s">
         <v>988</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C98" s="441" t="s">
+      <c r="C98" s="416" t="s">
         <v>989</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C99" s="441" t="s">
+      <c r="C99" s="416" t="s">
         <v>990</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C100" s="441" t="s">
+      <c r="C100" s="416" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C101" s="441" t="s">
+      <c r="C101" s="416" t="s">
         <v>992</v>
       </c>
     </row>
@@ -16480,12 +16666,12 @@
       <c r="B3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="427"/>
-      <c r="D3" s="427"/>
-      <c r="E3" s="427"/>
-      <c r="F3" s="427"/>
-      <c r="G3" s="427"/>
-      <c r="H3" s="428"/>
+      <c r="C3" s="429"/>
+      <c r="D3" s="429"/>
+      <c r="E3" s="429"/>
+      <c r="F3" s="429"/>
+      <c r="G3" s="429"/>
+      <c r="H3" s="430"/>
     </row>
     <row r="4" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
@@ -16533,12 +16719,12 @@
       <c r="H8" s="50"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="429"/>
-      <c r="D11" s="429"/>
-      <c r="E11" s="429"/>
-      <c r="F11" s="429"/>
-      <c r="G11" s="429"/>
-      <c r="H11" s="429"/>
+      <c r="C11" s="431"/>
+      <c r="D11" s="431"/>
+      <c r="E11" s="431"/>
+      <c r="F11" s="431"/>
+      <c r="G11" s="431"/>
+      <c r="H11" s="431"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C12" s="79"/>
@@ -16549,20 +16735,20 @@
       <c r="H12" s="79"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="429"/>
-      <c r="D13" s="429"/>
-      <c r="E13" s="429"/>
-      <c r="F13" s="429"/>
-      <c r="G13" s="429"/>
-      <c r="H13" s="429"/>
+      <c r="C13" s="431"/>
+      <c r="D13" s="431"/>
+      <c r="E13" s="431"/>
+      <c r="F13" s="431"/>
+      <c r="G13" s="431"/>
+      <c r="H13" s="431"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="429"/>
-      <c r="D14" s="429"/>
-      <c r="E14" s="429"/>
-      <c r="F14" s="429"/>
-      <c r="G14" s="429"/>
-      <c r="H14" s="429"/>
+      <c r="C14" s="431"/>
+      <c r="D14" s="431"/>
+      <c r="E14" s="431"/>
+      <c r="F14" s="431"/>
+      <c r="G14" s="431"/>
+      <c r="H14" s="431"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -16576,18 +16762,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E56EFC2-D53C-E94F-BE49-98CCC07AD8B8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
@@ -16760,6 +16934,559 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445286BE-3B1A-1A41-9991-F76C978696E0}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="10" width="20.5" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="443"/>
+      <c r="B1" s="443"/>
+      <c r="C1" s="443"/>
+      <c r="D1" s="446" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H1" s="446" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I1" s="446" t="s">
+        <v>1008</v>
+      </c>
+      <c r="J1" s="446" t="s">
+        <v>1009</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="L1" t="s">
+        <v>996</v>
+      </c>
+      <c r="M1" s="446" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F2" t="s">
+        <v>995</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F3" t="s">
+        <v>995</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F4" t="s">
+        <v>995</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E5" t="s">
+        <v>995</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E6" t="s">
+        <v>995</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E7" t="s">
+        <v>995</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" t="s">
+        <v>995</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>997</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" t="s">
+        <v>995</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>998</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" t="s">
+        <v>995</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1028</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="M11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" t="s">
+        <v>995</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>999</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="M12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" t="s">
+        <v>995</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>999</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" t="s">
+        <v>993</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E14" t="s">
+        <v>995</v>
+      </c>
+      <c r="F14" s="442" t="s">
+        <v>1028</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" t="s">
+        <v>995</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>1001</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" t="s">
+        <v>995</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1026</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18" t="s">
+        <v>995</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1028</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="442" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="442" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="442" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E21" s="442"/>
+      <c r="F21" s="442"/>
+      <c r="G21" s="442"/>
+      <c r="H21" s="28" t="s">
+        <v>1010</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J21" s="444"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I22" s="445"/>
+      <c r="J22" s="445"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C23" t="s">
+        <v>241</v>
+      </c>
+      <c r="H23" s="447" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I23" s="445"/>
+      <c r="J23" s="445"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>232</v>
+      </c>
+      <c r="C24" t="s">
+        <v>233</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>1012</v>
+      </c>
+      <c r="I24" s="442"/>
+      <c r="J24" s="442"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" t="s">
+        <v>221</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" t="s">
+        <v>245</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" t="s">
+        <v>994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
@@ -16768,7 +17495,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F34"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>